<commit_message>
Thay đổi time random và link share bài ngắn gọn
</commit_message>
<xml_diff>
--- a/01. FaceBook/01. Data/nhom_share.xlsx
+++ b/01. FaceBook/01. Data/nhom_share.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Makerting online\Sang\code\code_share\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Makerting online\Tool\01. FaceBook\01. Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9120"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9120"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="75">
   <si>
     <t>Group_hongNguyenThi</t>
   </si>
@@ -130,9 +130,6 @@
     <t>492401487499641</t>
   </si>
   <si>
-    <t>Group_copMapMap</t>
-  </si>
-  <si>
     <t>391037157727116</t>
   </si>
   <si>
@@ -248,16 +245,29 @@
   </si>
   <si>
     <t>603879913082562</t>
+  </si>
+  <si>
+    <t>hanhnhan7891@gmail.com</t>
+  </si>
+  <si>
+    <t>copmapmap22@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="14"/>
+      <color theme="10"/>
       <name val="Times New Roman"/>
       <family val="2"/>
     </font>
@@ -279,17 +289,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -568,477 +583,674 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B67"/>
+  <dimension ref="A1:C67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.453125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="38.1796875" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="27.7265625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.81640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="29.54296875" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>34</v>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>74</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C2" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C3" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
+      <c r="B5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C6" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C7" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C9" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C10" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
+      <c r="B12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
+      <c r="B13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
+      <c r="B14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B15" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C16" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C17" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B18" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C19" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C20" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B21" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C22" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B23" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C23" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C24" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C25" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C26" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C27" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C28" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C29" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C30" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B31" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C31" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C32" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A34" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C34" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B35" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B36" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B37" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C37" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B38" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C39" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B40" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C40" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C41" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C42" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+        <v>51</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C44" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A46" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C46" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C47" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="C48" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="C49" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+        <v>54</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="C51" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="C53" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="C54" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A56" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A56" s="2" t="s">
+      <c r="C56" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A57" s="2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A57" s="2" t="s">
+      <c r="C57" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A58" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A58" s="2" t="s">
+      <c r="C58" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A59" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A59" s="2" t="s">
+      <c r="C59" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A60" s="2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A60" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="C60" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="C61" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A63" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A63" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="C63" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="C64" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A65" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A66" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A67" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C1" r:id="rId1"/>
+    <hyperlink ref="A1" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
thêm tk hồng nguyễn thị
</commit_message>
<xml_diff>
--- a/01. FaceBook/01. Data/nhom_share.xlsx
+++ b/01. FaceBook/01. Data/nhom_share.xlsx
@@ -28,9 +28,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="75">
   <si>
-    <t>Group_hongNguyenThi</t>
-  </si>
-  <si>
     <t>118543634914894</t>
   </si>
   <si>
@@ -251,6 +248,9 @@
   </si>
   <si>
     <t>copmapmap22@gmail.com</t>
+  </si>
+  <si>
+    <t>hongnguyen12229@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -586,7 +586,7 @@
   <dimension ref="A1:C67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -599,658 +599,659 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="C1" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A65" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A66" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A67" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C1" r:id="rId1"/>
     <hyperlink ref="A1" r:id="rId2"/>
+    <hyperlink ref="B1" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
sửa lỗi tool share group
</commit_message>
<xml_diff>
--- a/01. FaceBook/01. Data/nhom_share.xlsx
+++ b/01. FaceBook/01. Data/nhom_share.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="85">
   <si>
     <t>118543634914894</t>
   </si>
@@ -251,6 +251,36 @@
   </si>
   <si>
     <t>hongnguyen12229@gmail.com</t>
+  </si>
+  <si>
+    <t>vinhquang13531@gmail.com</t>
+  </si>
+  <si>
+    <t>171076470160303</t>
+  </si>
+  <si>
+    <t>1209295105801230</t>
+  </si>
+  <si>
+    <t>616734738469807</t>
+  </si>
+  <si>
+    <t>1856620574550792</t>
+  </si>
+  <si>
+    <t>494023894278277</t>
+  </si>
+  <si>
+    <t>277314789020591</t>
+  </si>
+  <si>
+    <t>249978345123454</t>
+  </si>
+  <si>
+    <t>436038656468443</t>
+  </si>
+  <si>
+    <t>1362279090456478</t>
   </si>
 </sst>
 </file>
@@ -583,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C67"/>
+  <dimension ref="A1:D67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -594,10 +624,11 @@
     <col min="1" max="1" width="27.7265625" style="1" customWidth="1"/>
     <col min="2" max="2" width="31.81640625" style="2" customWidth="1"/>
     <col min="3" max="3" width="29.54296875" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="8.7265625" style="1"/>
+    <col min="4" max="4" width="27.08984375" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>73</v>
       </c>
@@ -607,8 +638,11 @@
       <c r="C1" s="3" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D1" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -618,8 +652,11 @@
       <c r="C2" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D2" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -629,8 +666,11 @@
       <c r="C3" s="2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D3" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>33</v>
       </c>
@@ -640,8 +680,11 @@
       <c r="C4" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D4" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>34</v>
       </c>
@@ -651,8 +694,11 @@
       <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D5" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>35</v>
       </c>
@@ -662,8 +708,11 @@
       <c r="C6" s="2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D6" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
@@ -673,8 +722,11 @@
       <c r="C7" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D7" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>36</v>
       </c>
@@ -684,8 +736,11 @@
       <c r="C8" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D8" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>37</v>
       </c>
@@ -695,8 +750,11 @@
       <c r="C9" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D9" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>30</v>
       </c>
@@ -706,8 +764,11 @@
       <c r="C10" s="2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D10" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>38</v>
       </c>
@@ -717,8 +778,11 @@
       <c r="C11" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D11" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>39</v>
       </c>
@@ -728,8 +792,11 @@
       <c r="C12" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D12" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>40</v>
       </c>
@@ -739,8 +806,11 @@
       <c r="C13" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D13" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>41</v>
       </c>
@@ -750,8 +820,11 @@
       <c r="C14" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D14" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>5</v>
       </c>
@@ -761,8 +834,11 @@
       <c r="C15" s="2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D15" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>21</v>
       </c>
@@ -772,8 +848,11 @@
       <c r="C16" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D16" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>42</v>
       </c>
@@ -783,8 +862,11 @@
       <c r="C17" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D17" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>18</v>
       </c>
@@ -794,8 +876,11 @@
       <c r="C18" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D18" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>43</v>
       </c>
@@ -805,8 +890,11 @@
       <c r="C19" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D19" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>20</v>
       </c>
@@ -816,8 +904,11 @@
       <c r="C20" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D20" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>3</v>
       </c>
@@ -827,8 +918,11 @@
       <c r="C21" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D21" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>17</v>
       </c>
@@ -838,8 +932,11 @@
       <c r="C22" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D22" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>44</v>
       </c>
@@ -849,8 +946,11 @@
       <c r="C23" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D23" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
@@ -860,8 +960,11 @@
       <c r="C24" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D24" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>15</v>
       </c>
@@ -871,8 +974,11 @@
       <c r="C25" s="2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D25" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>22</v>
       </c>
@@ -882,8 +988,11 @@
       <c r="C26" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D26" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>28</v>
       </c>
@@ -893,8 +1002,11 @@
       <c r="C27" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D27" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>19</v>
       </c>
@@ -904,8 +1016,11 @@
       <c r="C28" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D28" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>24</v>
       </c>
@@ -915,8 +1030,11 @@
       <c r="C29" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D29" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>25</v>
       </c>
@@ -926,8 +1044,11 @@
       <c r="C30" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D30" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>45</v>
       </c>
@@ -937,8 +1058,11 @@
       <c r="C31" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D31" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>8</v>
       </c>
@@ -948,8 +1072,11 @@
       <c r="C32" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D32" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>46</v>
       </c>
@@ -959,8 +1086,11 @@
       <c r="C33" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D33" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>47</v>
       </c>
@@ -970,8 +1100,11 @@
       <c r="C34" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D34" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>11</v>
       </c>
@@ -981,8 +1114,11 @@
       <c r="C35" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D35" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>12</v>
       </c>
@@ -992,8 +1128,11 @@
       <c r="C36" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D36" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>48</v>
       </c>
@@ -1003,8 +1142,11 @@
       <c r="C37" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D37" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>9</v>
       </c>
@@ -1014,8 +1156,11 @@
       <c r="C38" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D38" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
         <v>7</v>
       </c>
@@ -1025,8 +1170,11 @@
       <c r="C39" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D39" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
         <v>49</v>
       </c>
@@ -1036,120 +1184,165 @@
       <c r="C40" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D40" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D41" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D42" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
         <v>50</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D43" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D44" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
         <v>51</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D45" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
         <v>52</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D46" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D47" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D48" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D49" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
         <v>53</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D50" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D51" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
         <v>54</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D52" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D53" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D54" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" s="2" t="s">
         <v>55</v>
       </c>
@@ -1157,7 +1350,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
         <v>56</v>
       </c>
@@ -1165,7 +1358,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="2" t="s">
         <v>57</v>
       </c>
@@ -1173,7 +1366,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="2" t="s">
         <v>58</v>
       </c>
@@ -1181,7 +1374,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="2" t="s">
         <v>59</v>
       </c>
@@ -1189,7 +1382,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="2" t="s">
         <v>60</v>
       </c>
@@ -1197,7 +1390,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="2" t="s">
         <v>32</v>
       </c>
@@ -1205,7 +1398,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" s="2" t="s">
         <v>61</v>
       </c>
@@ -1213,7 +1406,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" s="2" t="s">
         <v>62</v>
       </c>
@@ -1221,7 +1414,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" s="2" t="s">
         <v>0</v>
       </c>
@@ -1249,9 +1442,10 @@
     <hyperlink ref="C1" r:id="rId1"/>
     <hyperlink ref="A1" r:id="rId2"/>
     <hyperlink ref="B1" r:id="rId3"/>
+    <hyperlink ref="D1" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
up data group thành phố
</commit_message>
<xml_diff>
--- a/01. FaceBook/01. Data/nhom_share.xlsx
+++ b/01. FaceBook/01. Data/nhom_share.xlsx
@@ -650,10 +650,10 @@
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -664,10 +664,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>20</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -678,10 +678,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -692,10 +692,10 @@
         <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -706,10 +706,10 @@
         <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -720,10 +720,10 @@
         <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>41</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -734,10 +734,10 @@
         <v>6</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>69</v>
+        <v>7</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
@@ -748,10 +748,10 @@
         <v>7</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -762,10 +762,10 @@
         <v>8</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>40</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -776,10 +776,10 @@
         <v>9</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -790,10 +790,10 @@
         <v>10</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>15</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
@@ -804,10 +804,10 @@
         <v>11</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>22</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
@@ -818,10 +818,10 @@
         <v>12</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
@@ -832,10 +832,10 @@
         <v>66</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>65</v>
+        <v>20</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>19</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
@@ -846,10 +846,10 @@
         <v>13</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>24</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
@@ -860,10 +860,10 @@
         <v>14</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
@@ -874,10 +874,10 @@
         <v>67</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>38</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
@@ -888,10 +888,10 @@
         <v>15</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
@@ -902,10 +902,10 @@
         <v>16</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
@@ -916,10 +916,10 @@
         <v>68</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>77</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
@@ -930,10 +930,10 @@
         <v>17</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>71</v>
+        <v>31</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
@@ -944,10 +944,10 @@
         <v>18</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>70</v>
+        <v>2</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
@@ -958,10 +958,10 @@
         <v>19</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
@@ -972,10 +972,10 @@
         <v>20</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>4</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
@@ -986,10 +986,10 @@
         <v>21</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
@@ -1000,10 +1000,10 @@
         <v>22</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
@@ -1014,10 +1014,10 @@
         <v>23</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
@@ -1028,10 +1028,10 @@
         <v>24</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>16</v>
+        <v>81</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
@@ -1042,10 +1042,10 @@
         <v>25</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>69</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
@@ -1056,10 +1056,10 @@
         <v>26</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>70</v>
+        <v>26</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
@@ -1070,10 +1070,10 @@
         <v>27</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
@@ -1084,10 +1084,10 @@
         <v>28</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
@@ -1098,10 +1098,10 @@
         <v>29</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>63</v>
+        <v>12</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>62</v>
+        <v>83</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
@@ -1112,10 +1112,10 @@
         <v>69</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
@@ -1126,10 +1126,10 @@
         <v>70</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
@@ -1140,10 +1140,10 @@
         <v>30</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
@@ -1154,10 +1154,10 @@
         <v>71</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
@@ -1168,10 +1168,10 @@
         <v>31</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
@@ -1182,10 +1182,10 @@
         <v>32</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>64</v>
+        <v>36</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
@@ -1193,10 +1193,10 @@
         <v>31</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
@@ -1204,10 +1204,10 @@
         <v>26</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
@@ -1215,10 +1215,10 @@
         <v>50</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>80</v>
+        <v>39</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
@@ -1226,10 +1226,10 @@
         <v>4</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
@@ -1237,10 +1237,10 @@
         <v>51</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
@@ -1248,10 +1248,10 @@
         <v>52</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
@@ -1259,10 +1259,10 @@
         <v>29</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>81</v>
+        <v>15</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
@@ -1270,10 +1270,10 @@
         <v>27</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
@@ -1281,10 +1281,10 @@
         <v>2</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
@@ -1292,10 +1292,10 @@
         <v>53</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>68</v>
+        <v>19</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
@@ -1303,10 +1303,10 @@
         <v>13</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>19</v>
+        <v>71</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>82</v>
+        <v>24</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
@@ -1314,10 +1314,10 @@
         <v>54</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
@@ -1325,10 +1325,10 @@
         <v>6</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
@@ -1336,10 +1336,10 @@
         <v>16</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>84</v>
+        <v>25</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
@@ -1347,7 +1347,7 @@
         <v>55</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>60</v>
+        <v>10</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
@@ -1355,7 +1355,7 @@
         <v>56</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
@@ -1363,7 +1363,7 @@
         <v>57</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>2</v>
+        <v>40</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
@@ -1371,7 +1371,7 @@
         <v>58</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
@@ -1379,7 +1379,7 @@
         <v>59</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
@@ -1387,7 +1387,7 @@
         <v>60</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
@@ -1395,7 +1395,7 @@
         <v>32</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
@@ -1403,7 +1403,7 @@
         <v>61</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
@@ -1411,7 +1411,7 @@
         <v>62</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>5</v>
+        <v>63</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
@@ -1419,7 +1419,7 @@
         <v>0</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
đổi via qua lại chạy
</commit_message>
<xml_diff>
--- a/01. FaceBook/01. Data/nhom_share.xlsx
+++ b/01. FaceBook/01. Data/nhom_share.xlsx
@@ -616,7 +616,7 @@
   <dimension ref="A1:D67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -650,10 +650,10 @@
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -664,10 +664,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -678,10 +678,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>3</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -692,10 +692,10 @@
         <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>30</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -706,10 +706,10 @@
         <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>64</v>
+        <v>19</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>36</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -720,10 +720,10 @@
         <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -734,10 +734,10 @@
         <v>6</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
@@ -748,10 +748,10 @@
         <v>7</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -762,10 +762,10 @@
         <v>8</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -776,10 +776,10 @@
         <v>9</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -790,10 +790,10 @@
         <v>10</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>59</v>
+        <v>2</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>69</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
@@ -804,10 +804,10 @@
         <v>11</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
@@ -818,10 +818,10 @@
         <v>12</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
@@ -832,10 +832,10 @@
         <v>66</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>78</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
@@ -846,10 +846,10 @@
         <v>13</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>62</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
@@ -860,10 +860,10 @@
         <v>14</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
@@ -874,10 +874,10 @@
         <v>67</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>68</v>
+        <v>5</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>79</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
@@ -888,10 +888,10 @@
         <v>15</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
@@ -902,10 +902,10 @@
         <v>16</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>17</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
@@ -916,10 +916,10 @@
         <v>68</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>7</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
@@ -930,10 +930,10 @@
         <v>17</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>8</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
@@ -944,10 +944,10 @@
         <v>18</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
@@ -958,10 +958,10 @@
         <v>19</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>12</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
@@ -972,10 +972,10 @@
         <v>20</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>80</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
@@ -986,10 +986,10 @@
         <v>21</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>55</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
@@ -1000,10 +1000,10 @@
         <v>22</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
@@ -1014,10 +1014,10 @@
         <v>23</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
@@ -1028,10 +1028,10 @@
         <v>24</v>
       </c>
       <c r="C29" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
@@ -1042,10 +1042,10 @@
         <v>25</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
@@ -1056,10 +1056,10 @@
         <v>26</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
@@ -1070,10 +1070,10 @@
         <v>27</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
@@ -1084,10 +1084,10 @@
         <v>28</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>82</v>
+        <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
@@ -1098,10 +1098,10 @@
         <v>29</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>83</v>
+        <v>44</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
@@ -1112,10 +1112,10 @@
         <v>69</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>61</v>
+        <v>28</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
@@ -1126,10 +1126,10 @@
         <v>70</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>84</v>
+        <v>22</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
@@ -1140,10 +1140,10 @@
         <v>30</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>69</v>
+        <v>21</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
@@ -1154,10 +1154,10 @@
         <v>71</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
@@ -1168,10 +1168,10 @@
         <v>31</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>58</v>
+        <v>29</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
@@ -1182,10 +1182,10 @@
         <v>32</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>36</v>
+        <v>71</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>6</v>
+        <v>76</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
@@ -1193,10 +1193,10 @@
         <v>31</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
@@ -1204,10 +1204,10 @@
         <v>26</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>51</v>
+        <v>15</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
@@ -1215,10 +1215,10 @@
         <v>50</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
@@ -1226,10 +1226,10 @@
         <v>4</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>42</v>
+        <v>77</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
@@ -1237,10 +1237,10 @@
         <v>51</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>40</v>
+        <v>3</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
@@ -1248,10 +1248,10 @@
         <v>52</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
@@ -1259,10 +1259,10 @@
         <v>29</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
@@ -1270,10 +1270,10 @@
         <v>27</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
@@ -1281,10 +1281,10 @@
         <v>2</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
@@ -1292,10 +1292,10 @@
         <v>53</v>
       </c>
       <c r="C50" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D50" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
@@ -1303,10 +1303,10 @@
         <v>13</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
@@ -1314,10 +1314,10 @@
         <v>54</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>76</v>
+        <v>16</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
@@ -1325,10 +1325,10 @@
         <v>6</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>38</v>
+        <v>69</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
@@ -1336,10 +1336,10 @@
         <v>16</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>67</v>
+        <v>9</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
@@ -1347,7 +1347,7 @@
         <v>55</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
@@ -1355,7 +1355,7 @@
         <v>56</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
@@ -1363,7 +1363,7 @@
         <v>57</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
@@ -1371,7 +1371,7 @@
         <v>58</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
@@ -1379,7 +1379,7 @@
         <v>59</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>18</v>
+        <v>57</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
@@ -1387,7 +1387,7 @@
         <v>60</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
@@ -1395,7 +1395,7 @@
         <v>32</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
@@ -1403,7 +1403,7 @@
         <v>61</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
@@ -1411,7 +1411,7 @@
         <v>62</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
@@ -1419,7 +1419,7 @@
         <v>0</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.35">

</xml_diff>